<commit_message>
still completed cpc for User1 QC
</commit_message>
<xml_diff>
--- a/DataSheet/CPC_1stTouchPoint_Approval.xlsx
+++ b/DataSheet/CPC_1stTouchPoint_Approval.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BSA_MOBILE_FRAMEWORK\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6E6ADB-5B8B-4F71-8D8E-9396525AD8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D05F93-0FB4-4083-85E6-832172E615C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{875AE543-1650-41B3-9C38-4B818EB686AA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{875AE543-1650-41B3-9C38-4B818EB686AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -562,7 +562,7 @@
     <t>(//button[text()='Proceed'])[2]</t>
   </si>
   <si>
-    <t>MF24121000006346</t>
+    <t>MF24121100006429</t>
   </si>
 </sst>
 </file>
@@ -958,7 +958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0CA32F-6895-4985-AF4D-119BC41D4938}">
   <dimension ref="A1:O294"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
+    <sheetView zoomScale="77" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -9264,8 +9264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A86AEA-BDCA-4ACF-93E7-52FBBDAF5EE7}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>